<commit_message>
Pushing 04/18/2024 work for merge
 On branch N5QC_20240418_2
 Changes to be committed:
	modified:   Lessons_and_Logs/Inventr_io/0-Getting_Started/Notes/Lesson_0_Notes_and_Journal.docx
	new file:   Lessons_and_Logs/Inventr_io/1-Traffic_Light_Simulator/CAD/Lesson_1.fzz
	new file:   Lessons_and_Logs/Inventr_io/1-Traffic_Light_Simulator/Notes/Lesson_1_Notes_and_Journal.docx
	modified:   Project_Management/2024_04_18_Python_Gantt_Schedule.xlsx
</commit_message>
<xml_diff>
--- a/Project_Management/2024_04_18_Python_Gantt_Schedule.xlsx
+++ b/Project_Management/2024_04_18_Python_Gantt_Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59805FCD-0DB1-43A3-865E-95858FAA13ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB2CDF2-5224-4D81-BAA0-E6A44F8C8F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1036,8 +1036,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Pushing 4/19/24 work -- Lesson 1
 On branch N5QC_20240419
 Changes to be committed:
	modified:   Lessons_and_Logs/Inventr_io/1-Traffic_Light_Simulator/CAD/Lesson_1.fzz
	new file:   Lessons_and_Logs/Inventr_io/1-Traffic_Light_Simulator/Notes/LED_Schematic_Note_1.pdf
	new file:   Lessons_and_Logs/Inventr_io/1-Traffic_Light_Simulator/Notes/Lesson_1_Code_Review.docx
	modified:   Lessons_and_Logs/Inventr_io/1-Traffic_Light_Simulator/Notes/Lesson_1_Notes_and_Journal.docx
	new file:   Lessons_and_Logs/Inventr_io/1-Traffic_Light_Simulator/Notes/Lesson_1_Verification_and_Troubleshooting.docx
	modified:   Project_Management/2024_04_18_Python_Gantt_Schedule.xlsx
	new file:   Project_Management/Supplemental_Activities.docx
</commit_message>
<xml_diff>
--- a/Project_Management/2024_04_18_Python_Gantt_Schedule.xlsx
+++ b/Project_Management/2024_04_18_Python_Gantt_Schedule.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB2CDF2-5224-4D81-BAA0-E6A44F8C8F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F7EF86-B5A7-4ED7-9BE7-9A76A45AE3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>PERIODS</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>KiCad Tutorial</t>
+  </si>
+  <si>
+    <t>Fritzig Tutorial</t>
   </si>
 </sst>
 </file>
@@ -1036,8 +1039,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1504,8 +1507,8 @@
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="6">
-        <v>2</v>
+      <c r="B13" s="6" t="s">
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <f>C12+D12</f>
@@ -1634,9 +1637,11 @@
       <c r="E20" s="7">
         <v>18</v>
       </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
       <c r="G20" s="8">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>